<commit_message>
Dinge ausprobiert und Variablen umbennat
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\MoBi\4. SS25\Data Analysis Project\2025-topic-03-group-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD09D252-A89B-4216-9858-B12F9940DCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E9D142-241D-495F-910C-814E9DD894BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Our equivalent names</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Variable names Maiwen</t>
+  </si>
+  <si>
+    <t>levels_CR</t>
+  </si>
+  <si>
+    <t>levels_fraction</t>
+  </si>
+  <si>
+    <t>fraction_names</t>
+  </si>
+  <si>
+    <t>colmns_sorted</t>
   </si>
 </sst>
 </file>
@@ -170,13 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -192,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -511,10 +524,10 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
@@ -540,7 +553,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -548,24 +561,24 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -588,8 +601,8 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Habe den Code schöner geschrieben
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E9D142-241D-495F-910C-814E9DD894BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA7FA97-1EB7-4E1A-830B-027928E2685F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="7860" yWindow="1368" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -182,11 +182,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F06AA-E558-4CA4-B5F5-8680A9E1BEF7}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +552,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -561,7 +560,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -569,7 +568,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -577,7 +576,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -601,7 +600,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Weiter mit Data cleanup gemacht
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA7FA97-1EB7-4E1A-830B-027928E2685F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627322B-C056-40A8-BE8E-6C696C385A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="1368" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Erklärung des Chunks ist drin
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627322B-C056-40A8-BE8E-6C696C385A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7451C735-A957-41C5-AFA6-6B23A3193269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="4548" yWindow="3492" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
   <si>
     <t>Our equivalent names</t>
   </si>
@@ -126,13 +126,695 @@
   </si>
   <si>
     <t>colmns_sorted</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Inhalt / Funktion</t>
+  </si>
+  <si>
+    <t>data.frame</t>
+  </si>
+  <si>
+    <t>Hauptdatentabelle</t>
+  </si>
+  <si>
+    <t>Zeilen = Proteine, Spalten = 150 Proben (25 Fraktionen × 6 Replikate)</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>Behandlungsgruppe je Spalte</t>
+  </si>
+  <si>
+    <t>"CTRL" oder "RNASE", jeweils 75 Wiederholungen</t>
+  </si>
+  <si>
+    <t>Replikatbezeichnung pro Spalte</t>
+  </si>
+  <si>
+    <t>"Ctrl_Rep1", ..., "RNase_Rep3", 25 Wiederholungen</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>Fraktionsbezeichnung pro Spalte</t>
+  </si>
+  <si>
+    <t>"fraction1" bis "fraction25", jeweils 6 Wiederholungen</t>
+  </si>
+  <si>
+    <t>Metadaten der Spalten</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spalten = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>levels_CR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>levels_fraction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>fraction_names</t>
+    </r>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Anzahl Proteine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anzahl Zeilen von </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NS_Table</t>
+    </r>
+  </si>
+  <si>
+    <t>Namen der Proteine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zeilennamen von </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NS_Table</t>
+    </r>
+  </si>
+  <si>
+    <t>fraction.tables</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Unterteilung nach Fraktionen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">25 Einträge: jede ein </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>data.frame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mit 6 Spalten (3 CTRL + 3 RNASE)</t>
+    </r>
+  </si>
+  <si>
+    <t>selected_proteins</t>
+  </si>
+  <si>
+    <t>Namen der Fraktionen</t>
+  </si>
+  <si>
+    <t>"fraction1" bis "fraction25"</t>
+  </si>
+  <si>
+    <t>fraction.tables.CTRL</t>
+  </si>
+  <si>
+    <t>Nur CTRL-Spalten je Fraktion</t>
+  </si>
+  <si>
+    <t>Je 3 Spalten pro Fraktion</t>
+  </si>
+  <si>
+    <t>fraction.tables.RNASE</t>
+  </si>
+  <si>
+    <t>Nur RNASE-Spalten je Fraktion</t>
+  </si>
+  <si>
+    <t>avg.tables.CTRL</t>
+  </si>
+  <si>
+    <t>Mittelwerte der Replikate (CTRL)</t>
+  </si>
+  <si>
+    <t>Vektor mit 3 Werten je Fraktion</t>
+  </si>
+  <si>
+    <t>avg.tables.RNASE</t>
+  </si>
+  <si>
+    <t>Mittelwerte der Replikate (RNASE)</t>
+  </si>
+  <si>
+    <t>Analog zu oben</t>
+  </si>
+  <si>
+    <t>norm_fact()</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>Robustmittelwert der 2 ähnlichsten Replikate</t>
+  </si>
+  <si>
+    <t>Gibt Mittelwert der 2 ähnlichsten Werte von 3</t>
+  </si>
+  <si>
+    <t>norm_mean_frxn_CTRL</t>
+  </si>
+  <si>
+    <t>Normierungsfaktoren (CTRL)</t>
+  </si>
+  <si>
+    <t>Vektor: normierter Mittelwert geteilt durch einzelne Replikatwerte</t>
+  </si>
+  <si>
+    <t>norm_mean_frxn_RNASE</t>
+  </si>
+  <si>
+    <t>Normierungsfaktoren (RNASE)</t>
+  </si>
+  <si>
+    <t>Siehe oben</t>
+  </si>
+  <si>
+    <r>
+      <t>norm.ctrl1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>norm.ctrl3</t>
+    </r>
+  </si>
+  <si>
+    <t>Normierungsvektoren für CTRL Replikate</t>
+  </si>
+  <si>
+    <t>Vektor mit 25 Werten</t>
+  </si>
+  <si>
+    <r>
+      <t>norm.rnase1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>norm.rnase3</t>
+    </r>
+  </si>
+  <si>
+    <t>Normierungsvektoren für RNASE Replikate</t>
+  </si>
+  <si>
+    <r>
+      <t>data.ctrl1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>data.rnase3</t>
+    </r>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>Selektor für Spalten</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE je nachdem ob Spalte zu Replikat gehört</t>
+  </si>
+  <si>
+    <t>normalize_group()</t>
+  </si>
+  <si>
+    <t>Multipliziert ausgewählte Spalten mit Normierungsvektor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gibt normalisierten </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>data.frame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zurück</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>table.ctrl1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>table.rnase3</t>
+    </r>
+  </si>
+  <si>
+    <t>Ergebnis nach fraktionsweiser Normalisierung</t>
+  </si>
+  <si>
+    <t>Proteine × 25 Fraktionen, normalisiert</t>
+  </si>
+  <si>
+    <t>smooth_table()</t>
+  </si>
+  <si>
+    <t>Gleitender Mittelwert mit Fenstergröße 3</t>
+  </si>
+  <si>
+    <t>Verwendet für Fraktionsglättung</t>
+  </si>
+  <si>
+    <r>
+      <t>table.ctrl1.SW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.SW</t>
+    </r>
+  </si>
+  <si>
+    <t>Nach Glättung mit Moving Average</t>
+  </si>
+  <si>
+    <t>Gleiche Dimension wie vorher</t>
+  </si>
+  <si>
+    <t>normalize_table()</t>
+  </si>
+  <si>
+    <t>Normalisiert jede Zeile auf Summe 100</t>
+  </si>
+  <si>
+    <t>Zeilensumme = 100</t>
+  </si>
+  <si>
+    <r>
+      <t>norm_tables.ctrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.rnase</t>
+    </r>
+  </si>
+  <si>
+    <t>Tabellen mit 100%-Normalisierung</t>
+  </si>
+  <si>
+    <t>Für alle 3 Replikate</t>
+  </si>
+  <si>
+    <t>clean_table()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ersetzt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NaN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> durch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>Für bereinigte Tabellen</t>
+  </si>
+  <si>
+    <r>
+      <t>tables.norm.ctrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.rnase</t>
+    </r>
+  </si>
+  <si>
+    <t>Bereinigte normierte Tabellen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enthält </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ctrl1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ctrl3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bzw. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>rnase1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>rnase3</t>
+    </r>
+  </si>
+  <si>
+    <t>my.list.ctrl.norm</t>
+  </si>
+  <si>
+    <t>Enthält geglättete Tabellen vor finaler 100%-Normierung</t>
+  </si>
+  <si>
+    <t>ctrl1.SW bis ctrl3.SW</t>
+  </si>
+  <si>
+    <t>ctrl_norm_mean</t>
+  </si>
+  <si>
+    <t>Mittelwert über alle CTRL-Replikate</t>
+  </si>
+  <si>
+    <t>Resultierende Normalisierungstabelle</t>
+  </si>
+  <si>
+    <t>rnase_norm_mean</t>
+  </si>
+  <si>
+    <t>Mittelwert über alle RNASE-Replikate</t>
+  </si>
+  <si>
+    <t>Wie oben, aber für RNASE</t>
+  </si>
+  <si>
+    <t>replace_na_nan()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ersetzt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NaN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in Datenrahmen</t>
+    </r>
+  </si>
+  <si>
+    <t>Auf finalen Tabellen angewendet</t>
+  </si>
+  <si>
+    <t>Namen der Fraktionsspalten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +836,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -182,10 +877,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,213 +1224,631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F06AA-E558-4CA4-B5F5-8680A9E1BEF7}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" customWidth="1"/>
+    <col min="7" max="7" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="100.8">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="86.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="86.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="82.8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="42">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="86.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="72">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="100.8">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="57.6">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="72">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="72">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="86.4">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="57.6">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="43.2">
+      <c r="D25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.6">
+      <c r="D26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="43.2">
+      <c r="D27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="70.8">
+      <c r="D28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="72">
+      <c r="D29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="57.6">
+      <c r="D30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.6">
+      <c r="D31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="57.6">
+      <c r="D32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" ht="43.2">
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Teil 3 funktioniert jetzt
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7451C735-A957-41C5-AFA6-6B23A3193269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E246E8D-2572-490A-A09E-1000751A0EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4548" yWindow="3492" windowWidth="17280" windowHeight="9960" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
   <si>
     <t>Our equivalent names</t>
   </si>
@@ -808,6 +808,9 @@
   </si>
   <si>
     <t>Namen der Fraktionsspalten</t>
+  </si>
+  <si>
+    <t>table.ctrl1.SW.norm</t>
   </si>
 </sst>
 </file>
@@ -1226,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F06AA-E558-4CA4-B5F5-8680A9E1BEF7}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -1240,7 +1243,7 @@
     <col min="7" max="7" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="100.8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="72">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="86.4">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="86.4">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="82.8">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="86.4">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1480,7 +1483,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="100.8">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57.6">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57.6">
+    <row r="19" spans="1:7" ht="27.6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="72">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="72">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="86.4">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="72">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="57.6">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2">
+    <row r="25" spans="1:7">
       <c r="D25" s="5" t="s">
         <v>101</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57.6">
+    <row r="26" spans="1:7">
       <c r="D26" s="5" t="s">
         <v>104</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.2">
+    <row r="27" spans="1:7">
       <c r="D27" s="5" t="s">
         <v>107</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="70.8">
+    <row r="28" spans="1:7">
       <c r="D28" s="5" t="s">
         <v>110</v>
       </c>
@@ -1776,7 +1779,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="72">
+    <row r="29" spans="1:7">
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>113</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="57.6">
+    <row r="30" spans="1:7">
       <c r="D30" s="5" t="s">
         <v>116</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="57.6">
+    <row r="31" spans="1:7">
       <c r="D31" s="5" t="s">
         <v>119</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="57.6">
+    <row r="32" spans="1:7">
       <c r="D32" s="5" t="s">
         <v>122</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="4:7" ht="43.2">
+    <row r="33" spans="4:7">
       <c r="D33" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Versuch vom Proportion test
</commit_message>
<xml_diff>
--- a/Variable_names_overview.xlsx
+++ b/Variable_names_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_n\Documents\GitHub\2025-topic-03-group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E246E8D-2572-490A-A09E-1000751A0EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3809E2C2-9E5A-4A0B-BF88-2EC5961A8C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{8CE5977E-1E95-472E-BCDC-9A1AB8EBC7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="156">
   <si>
     <t>Our equivalent names</t>
   </si>
@@ -810,7 +810,94 @@
     <t>Namen der Fraktionsspalten</t>
   </si>
   <si>
-    <t>table.ctrl1.SW.norm</t>
+    <t>Inhalt von ctrl_mean_filtert_final</t>
+  </si>
+  <si>
+    <t>Bedeutung</t>
+  </si>
+  <si>
+    <t>pb_fit</t>
+  </si>
+  <si>
+    <t>sum_area</t>
+  </si>
+  <si>
+    <t>fit_area</t>
+  </si>
+  <si>
+    <t>fit_c_fxn</t>
+  </si>
+  <si>
+    <t>fit_mean_fxn</t>
+  </si>
+  <si>
+    <t>fit_param</t>
+  </si>
+  <si>
+    <t>fitted</t>
+  </si>
+  <si>
+    <t>fit_res</t>
+  </si>
+  <si>
+    <t>fit_sigma</t>
+  </si>
+  <si>
+    <t>nb_max</t>
+  </si>
+  <si>
+    <t>ctrl_max</t>
+  </si>
+  <si>
+    <t>peaks</t>
+  </si>
+  <si>
+    <t>maxima</t>
+  </si>
+  <si>
+    <t>Anzahl lokale Maxima</t>
+  </si>
+  <si>
+    <t>gibt es zusätzlich zum Hochpunkt ein Platteau</t>
+  </si>
+  <si>
+    <t>Koordinate lokaler Maxima</t>
+  </si>
+  <si>
+    <t>Koordinate lokaler Maxima und Platteaus</t>
+  </si>
+  <si>
+    <t>Amplitude der Punkte</t>
+  </si>
+  <si>
+    <t>Mittelwert der Punkte</t>
+  </si>
+  <si>
+    <t>Standardabweichung der Punkte</t>
+  </si>
+  <si>
+    <t>reseduals sum of squares</t>
+  </si>
+  <si>
+    <t>Checkt, ob eine gefittete Kurve gefunden wurde</t>
+  </si>
+  <si>
+    <t>Die Amplitude, Mittelwert und Standard Abweichung werden den Hochpunkten zugeordnet</t>
+  </si>
+  <si>
+    <t>Mittelwert der Punkte nur Ränder werden mit einebzogen</t>
+  </si>
+  <si>
+    <t>Amplitude der Punkte nur Ränder werden mit einebzogen</t>
+  </si>
+  <si>
+    <t>Area unter jedem Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Summe der Areas</t>
+  </si>
+  <si>
+    <t>Checkt, ob Kurve fittet</t>
   </si>
 </sst>
 </file>
@@ -1227,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F06AA-E558-4CA4-B5F5-8680A9E1BEF7}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -1238,7 +1325,8 @@
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
     <col min="6" max="6" width="49.109375" customWidth="1"/>
     <col min="7" max="7" width="56.6640625" customWidth="1"/>
   </cols>
@@ -1780,9 +1868,6 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" t="s">
-        <v>126</v>
-      </c>
       <c r="D29" s="5" t="s">
         <v>113</v>
       </c>
@@ -1850,6 +1935,134 @@
       </c>
       <c r="G33" s="4" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7">
+      <c r="D41" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7">
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7">
+      <c r="D43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7">
+      <c r="D44" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7">
+      <c r="D45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7">
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7">
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7">
+      <c r="D48" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5">
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5">
+      <c r="D54" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5">
+      <c r="D55" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5">
+      <c r="D56" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>